<commit_message>
Minor changes to fix errors in amount of missing data
</commit_message>
<xml_diff>
--- a/data_clean.xlsx
+++ b/data_clean.xlsx
@@ -1117,10 +1117,10 @@
         </is>
       </c>
       <c r="AC3">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="AE3">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="AF3" t="inlineStr">
         <is>
@@ -3257,10 +3257,10 @@
         </is>
       </c>
       <c r="AH11">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="AJ11">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="AK11" t="inlineStr">
         <is>
@@ -7217,10 +7217,10 @@
         </is>
       </c>
       <c r="AC26">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="AE26">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="AF26" t="inlineStr">
         <is>
@@ -10167,10 +10167,10 @@
         </is>
       </c>
       <c r="AC37">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="AE37">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="AF37" t="inlineStr">
         <is>
@@ -11480,10 +11480,10 @@
         </is>
       </c>
       <c r="AC42">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="AE42">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="AF42" t="inlineStr">
         <is>
@@ -14449,10 +14449,10 @@
         </is>
       </c>
       <c r="AC53">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="AE53">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="AF53" t="inlineStr">
         <is>
@@ -16597,10 +16597,10 @@
         </is>
       </c>
       <c r="AC61">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="AE61">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="AF61" t="inlineStr">
         <is>
@@ -31963,14 +31963,14 @@
       </c>
       <c r="AB118" t="inlineStr">
         <is>
-          <t>Able to establish an upper bound only</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="AC118">
-        <v>13</v>
-      </c>
-      <c r="AE118">
-        <v>13</v>
+        <v>85</v>
+      </c>
+      <c r="AD118">
+        <v>85</v>
       </c>
       <c r="AF118" t="inlineStr">
         <is>
@@ -33587,14 +33587,8 @@
       </c>
       <c r="AL124" t="inlineStr">
         <is>
-          <t>Yes, but only able to establish a lower bound on the percentage of missing values</t>
-        </is>
-      </c>
-      <c r="AM124">
-        <v>81</v>
-      </c>
-      <c r="AO124">
-        <v>81</v>
+          <t>Yes, but unable to establish the percentage of missing values</t>
+        </is>
       </c>
       <c r="AP124" t="inlineStr">
         <is>

</xml_diff>